<commit_message>
arquivo de sacado mudado
</commit_message>
<xml_diff>
--- a/lib/xlsx_reader/CadastroSacados.xlsx
+++ b/lib/xlsx_reader/CadastroSacados.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CadastroSacados!$A$3:$H$445</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -6735,8 +6735,8 @@
   <dimension ref="A1:H445"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A85" sqref="A85:XFD85"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -16786,11 +16786,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:H445">
-    <sortState ref="A4:H445">
-      <sortCondition ref="A3:A445"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A3:H445"/>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>

</xml_diff>